<commit_message>
Module 5: add staticmethods for get/display functions and refactor, add functionality for get/display courses
</commit_message>
<xml_diff>
--- a/course.xlsx
+++ b/course.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8090a3a5aa513dda/Desktop/DATA 200/Assignments/Data200-Lab1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C7526A5B-357E-4E80-9543-6EF51666DDFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{C7526A5B-357E-4E80-9543-6EF51666DDFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E4F49861-C1C0-4578-A8EF-7647BCD77968}"/>
   <bookViews>
-    <workbookView xWindow="41955" yWindow="2310" windowWidth="19200" windowHeight="11715" xr2:uid="{429879E9-E5C7-48D7-BAE5-EB5DFFEC8E87}"/>
+    <workbookView xWindow="40110" yWindow="1710" windowWidth="21600" windowHeight="11175" xr2:uid="{429879E9-E5C7-48D7-BAE5-EB5DFFEC8E87}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>course_id</t>
   </si>
@@ -46,6 +46,15 @@
   </si>
   <si>
     <t>Utilizing Python in Data Science</t>
+  </si>
+  <si>
+    <t>DATA201</t>
+  </si>
+  <si>
+    <t>Intro to Databases</t>
+  </si>
+  <si>
+    <t>Utilizing SQL in Data Science</t>
   </si>
 </sst>
 </file>
@@ -417,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{142FD706-35DE-4146-AC96-1C3072365824}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -459,6 +468,20 @@
         <v>6</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>